<commit_message>
implemented date and date difference feature
</commit_message>
<xml_diff>
--- a/Reports/sourceFileName1.xlsx
+++ b/Reports/sourceFileName1.xlsx
@@ -7,6 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="sourceFileName1" r:id="rId3" sheetId="1"/>
+    <sheet name="Color Code Table" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -18,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -26,8 +27,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="16"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="16"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -66,16 +107,6 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
         <fgColor indexed="29"/>
       </patternFill>
     </fill>
@@ -86,16 +117,6 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
         <fgColor indexed="22"/>
       </patternFill>
     </fill>
@@ -106,16 +127,6 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="23"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="23"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
         <fgColor indexed="26"/>
       </patternFill>
     </fill>
@@ -126,12 +137,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="43"/>
+        <fgColor indexed="9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="43"/>
+        <fgColor indexed="9"/>
       </patternFill>
     </fill>
   </fills>
@@ -165,18 +176,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -227,12 +247,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Source_sourceHeader2</t>
+          <t>Source_sourceHeader3</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Target_targetHeader2</t>
+          <t>Target_targetHeader3</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -272,32 +292,32 @@
           <t>ejioru</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="F2" s="4" t="inlineStr">
         <is>
           <t>ioeurio</t>
         </is>
       </c>
-      <c r="G2" s="3" t="inlineStr">
+      <c r="G2" s="4" t="inlineStr">
         <is>
           <t>ioeurio</t>
         </is>
       </c>
       <c r="H2" s="5" t="inlineStr">
         <is>
-          <t>hfjhhjg</t>
+          <t>hjjfhhd</t>
         </is>
       </c>
       <c r="I2" s="5" t="inlineStr">
         <is>
-          <t>hfjjg</t>
-        </is>
-      </c>
-      <c r="J2" s="3" t="inlineStr">
+          <t>hfhhd</t>
+        </is>
+      </c>
+      <c r="J2" s="4" t="inlineStr">
         <is>
           <t>ihh</t>
         </is>
       </c>
-      <c r="K2" s="3" t="inlineStr">
+      <c r="K2" s="4" t="inlineStr">
         <is>
           <t>ihh</t>
         </is>
@@ -329,32 +349,32 @@
           <t>hjerj</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="F3" s="4" t="inlineStr">
         <is>
           <t>bjehjk</t>
         </is>
       </c>
-      <c r="G3" s="3" t="inlineStr">
+      <c r="G3" s="4" t="inlineStr">
         <is>
           <t>bjehjk</t>
         </is>
       </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
-          <t>iojehjro</t>
+          <t>jkreklj</t>
         </is>
       </c>
       <c r="I3" s="5" t="inlineStr">
         <is>
-          <t>iojehro</t>
-        </is>
-      </c>
-      <c r="J3" s="3" t="inlineStr">
+          <t>jeklj</t>
+        </is>
+      </c>
+      <c r="J3" s="4" t="inlineStr">
         <is>
           <t>iuoerh</t>
         </is>
       </c>
-      <c r="K3" s="3" t="inlineStr">
+      <c r="K3" s="4" t="inlineStr">
         <is>
           <t>iuoerh</t>
         </is>
@@ -388,37 +408,37 @@
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>header5</t>
+          <t>2022/12/12 05:30:00</t>
         </is>
       </c>
       <c r="G4" s="3" t="inlineStr">
         <is>
-          <t>header5</t>
+          <t>2022-12-12 00:00:00</t>
         </is>
       </c>
       <c r="H4" s="3" t="inlineStr">
         <is>
-          <t>header2</t>
+          <t>header3</t>
         </is>
       </c>
       <c r="I4" s="3" t="inlineStr">
         <is>
-          <t>header2</t>
-        </is>
-      </c>
-      <c r="J4" s="3" t="inlineStr">
+          <t>header3</t>
+        </is>
+      </c>
+      <c r="J4" s="4" t="inlineStr">
         <is>
           <t>header1</t>
         </is>
       </c>
-      <c r="K4" s="3" t="inlineStr">
+      <c r="K4" s="4" t="inlineStr">
         <is>
           <t>header1</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="inlineStr">
+      <c r="A5" s="7" t="inlineStr">
         <is>
           <t>Record is not present in Target CSV</t>
         </is>
@@ -455,7 +475,7 @@
       </c>
       <c r="H5" s="7" t="inlineStr">
         <is>
-          <t>iojehjro</t>
+          <t>jkreklj</t>
         </is>
       </c>
       <c r="I5" s="7" t="inlineStr">
@@ -475,47 +495,195 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="inlineStr">
+      <c r="A6" s="8" t="inlineStr">
         <is>
           <t>Record is not present in Source CSV</t>
         </is>
       </c>
-      <c r="B6" s="9" t="inlineStr">
-        <is>
-          <t>Record not Found</t>
-        </is>
-      </c>
-      <c r="C6" s="9" t="inlineStr">
+      <c r="B6" s="8" t="inlineStr">
+        <is>
+          <t>Record not Found</t>
+        </is>
+      </c>
+      <c r="C6" s="8" t="inlineStr">
         <is>
           <t>ExtraTargetRecord</t>
         </is>
       </c>
-      <c r="D6" s="9" t="inlineStr">
-        <is>
-          <t>Record not Found</t>
-        </is>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9" t="inlineStr">
-        <is>
-          <t>Record not Found</t>
-        </is>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9" t="inlineStr">
-        <is>
-          <t>Record not Found</t>
-        </is>
-      </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9" t="inlineStr">
-        <is>
-          <t>Record not Found</t>
-        </is>
-      </c>
-      <c r="K6" s="9"/>
+      <c r="D6" s="8" t="inlineStr">
+        <is>
+          <t>Record not Found</t>
+        </is>
+      </c>
+      <c r="E6" s="8" t="inlineStr">
+        <is>
+          <t>ejioru</t>
+        </is>
+      </c>
+      <c r="F6" s="8" t="inlineStr">
+        <is>
+          <t>Record not Found</t>
+        </is>
+      </c>
+      <c r="G6" s="8" t="inlineStr">
+        <is>
+          <t>ioeurio</t>
+        </is>
+      </c>
+      <c r="H6" s="8" t="inlineStr">
+        <is>
+          <t>Record not Found</t>
+        </is>
+      </c>
+      <c r="I6" s="8" t="inlineStr">
+        <is>
+          <t>hfhhd</t>
+        </is>
+      </c>
+      <c r="J6" s="8" t="inlineStr">
+        <is>
+          <t>Record not Found</t>
+        </is>
+      </c>
+      <c r="K6" s="8" t="inlineStr">
+        <is>
+          <t>ihh</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="B2:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="2">
+      <c r="B2" s="9" t="inlineStr">
+        <is>
+          <t>Color Code Table</t>
+        </is>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3">
+      <c r="B3" s="10" t="inlineStr">
+        <is>
+          <t>Priority Order</t>
+        </is>
+      </c>
+      <c r="C3" s="10" t="inlineStr">
+        <is>
+          <t>Cell Style</t>
+        </is>
+      </c>
+      <c r="D3" s="10" t="inlineStr">
+        <is>
+          <t>Style Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="12" t="inlineStr">
+        <is>
+          <t>Source Missing</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="inlineStr">
+        <is>
+          <t>The Records Present in Target CSV is not Present in Source CSV. (Extra Target Records)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="11" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C5" s="13" t="inlineStr">
+        <is>
+          <t>Target Missing</t>
+        </is>
+      </c>
+      <c r="D5" s="11" t="inlineStr">
+        <is>
+          <t>The Records Present in Source CSV is not Present in Target CSV. (Extra Source Records)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6" s="14" t="inlineStr">
+        <is>
+          <t>Mismatch and Invalid Date Format</t>
+        </is>
+      </c>
+      <c r="D6" s="11" t="inlineStr">
+        <is>
+          <t>There is mismatch between Source and Target Property and also date format are not matching with the format specified in the properties file</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="11" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C7" s="15" t="inlineStr">
+        <is>
+          <t>Mismatch</t>
+        </is>
+      </c>
+      <c r="D7" s="11" t="inlineStr">
+        <is>
+          <t>There is mismatch between Source and Target Property.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="11" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C8" s="16" t="inlineStr">
+        <is>
+          <t>Match and Invalid Date format</t>
+        </is>
+      </c>
+      <c r="D8" s="11" t="inlineStr">
+        <is>
+          <t>Matched but Date format not matching with specified format in property file</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="11" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C9" s="17" t="inlineStr">
+        <is>
+          <t>Match</t>
+        </is>
+      </c>
+      <c r="D9" s="11" t="inlineStr">
+        <is>
+          <t>Matched</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>